<commit_message>
fix 12.06.2025 18h + 27
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRVSteam_ver.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRVSteam_ver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Документы\ТЗ программа подбора TRV, RDT\ТЗ клапаны TRV\27.05.2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F11865-4643-42BC-892B-9BD4CCC75076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD4B365-93F5-4250-AC3F-6081145F8781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="1680" windowWidth="12765" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -298,80 +298,80 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -711,7 +711,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="I15" sqref="I15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,10 +721,10 @@
     <col min="3" max="5" width="7.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8" style="3" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="9" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="3" customWidth="1"/>
     <col min="12" max="23" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -737,12 +737,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="19"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="9"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -784,21 +784,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="22" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="27"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -813,12 +813,12 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -840,19 +840,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -867,18 +867,18 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="6"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -894,18 +894,18 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="6" t="s">
         <v>11</v>
       </c>
@@ -923,18 +923,18 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -950,13 +950,13 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -977,12 +977,12 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="10"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1004,12 +1004,12 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="10"/>
       <c r="F12" s="11"/>
       <c r="G12" s="11"/>
@@ -1056,23 +1056,23 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="29" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="29" t="s">
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J14" s="30"/>
-      <c r="K14" s="31"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1087,17 +1087,17 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="15"/>
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1112,19 +1112,19 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1970,18 +1970,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:K6"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="A8:H8"/>
     <mergeCell ref="A16:K16"/>
@@ -1998,6 +1986,18 @@
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="E11:K11"/>
     <mergeCell ref="E12:K12"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:K6"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix 20.06.2025 price 18h + 35h
</commit_message>
<xml_diff>
--- a/TeplosilaWeb/Content/templates/templateTRVSteam_ver.xlsx
+++ b/TeplosilaWeb/Content/templates/templateTRVSteam_ver.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pge27\OneDrive\Рабочий стол\TeploSilaWeb\TeplosilaWeb\Content\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD4B365-93F5-4250-AC3F-6081145F8781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8880B13B-AC27-4C48-ADD3-529BDF456A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Марка регулирующего клапана</t>
   </si>
   <si>
     <t>Скорость в выходном сечении клапана V, м/с</t>
-  </si>
-  <si>
-    <t>Шум, некачественное регулирование</t>
   </si>
   <si>
     <t>Дата расчета:</t>
@@ -98,6 +95,13 @@
   </si>
   <si>
     <t>Оптимальная скорость в выходном сечении клапана: 40 м/с для насыщенного пара; 60 м/с для перегретого пара.</t>
+  </si>
+  <si>
+    <t>Шум,
+некачественное регулирование</t>
+  </si>
+  <si>
+    <t>Давление пара после клапана (изб.) P'2, бар</t>
   </si>
 </sst>
 </file>
@@ -282,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,6 +302,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -307,21 +338,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -347,30 +363,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -711,7 +703,7 @@
   <dimension ref="A1:W50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:K15"/>
+      <selection activeCell="G15" sqref="G15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,12 +711,12 @@
     <col min="1" max="1" width="16.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" style="3" customWidth="1"/>
     <col min="3" max="5" width="7.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="8.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9" style="3" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" style="3" customWidth="1"/>
     <col min="12" max="23" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -737,12 +729,12 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7" t="s">
-        <v>3</v>
+      <c r="H2" s="16" t="s">
+        <v>2</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -758,18 +750,18 @@
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -784,21 +776,21 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>5</v>
+      <c r="A4" s="19" t="s">
+        <v>4</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17" t="s">
-        <v>12</v>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21" t="s">
+        <v>11</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -813,12 +805,12 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>6</v>
+      <c r="A5" s="27" t="s">
+        <v>5</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -840,19 +832,19 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>7</v>
+      <c r="A6" s="19" t="s">
+        <v>6</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -867,18 +859,18 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>13</v>
+      <c r="A7" s="7" t="s">
+        <v>12</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
       <c r="K7" s="6"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -894,20 +886,20 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>14</v>
+      <c r="A8" s="7" t="s">
+        <v>13</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
       <c r="K8" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -923,18 +915,18 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>15</v>
+      <c r="A9" s="7" t="s">
+        <v>14</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
       <c r="K9" s="6"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -950,13 +942,13 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
-        <v>8</v>
+      <c r="A10" s="12" t="s">
+        <v>7</v>
       </c>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -977,19 +969,19 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13" t="s">
-        <v>9</v>
+      <c r="A11" s="7" t="s">
+        <v>8</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="12"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1004,19 +996,19 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13" t="s">
-        <v>10</v>
+      <c r="A12" s="7" t="s">
+        <v>9</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="12"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1056,23 +1048,25 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" s="1" customFormat="1" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="24" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="24" t="s">
-        <v>2</v>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
+        <v>16</v>
       </c>
-      <c r="J14" s="25"/>
-      <c r="K14" s="26"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1087,17 +1081,17 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="30"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1112,19 +1106,19 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
-        <v>16</v>
+      <c r="A16" s="8" t="s">
+        <v>15</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1969,23 +1963,9 @@
       <c r="W50" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A16:K16"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="I14:K14"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="E11:K11"/>
-    <mergeCell ref="E12:K12"/>
+  <mergeCells count="30">
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:K3"/>
@@ -1998,6 +1978,22 @@
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:K6"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="I14:K14"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="E11:K11"/>
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>